<commit_message>
updated AOP AQU site availability
</commit_message>
<xml_diff>
--- a/data_availability/all_status.xlsx
+++ b/data_availability/all_status.xlsx
@@ -6758,61 +6758,61 @@
       <c r="D21" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="J21" t="s">
-        <v>132</v>
-      </c>
-      <c r="K21" t="s">
-        <v>132</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="M21" t="s">
-        <v>87</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="O21" t="s">
-        <v>87</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="S21" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="U21" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="V21" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="W21" t="s">
+      <c r="E21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" t="s">
+        <v>131</v>
+      </c>
+      <c r="H21" t="s">
+        <v>131</v>
+      </c>
+      <c r="I21" t="s">
+        <v>131</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L21" t="s">
+        <v>88</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="N21" t="s">
+        <v>88</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P21" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>88</v>
+      </c>
+      <c r="R21" t="s">
+        <v>88</v>
+      </c>
+      <c r="S21" t="s">
+        <v>88</v>
+      </c>
+      <c r="T21" t="s">
+        <v>88</v>
+      </c>
+      <c r="U21" t="s">
+        <v>88</v>
+      </c>
+      <c r="V21" t="s">
+        <v>88</v>
+      </c>
+      <c r="W21" s="1" t="s">
         <v>87</v>
       </c>
       <c r="X21" t="s">
@@ -6827,13 +6827,13 @@
       <c r="AA21" t="s">
         <v>87</v>
       </c>
-      <c r="AB21" t="s">
+      <c r="AB21" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC21" t="s">
         <v>91</v>
       </c>
-      <c r="AD21" t="s">
+      <c r="AD21" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AE21" t="s">
@@ -6842,10 +6842,10 @@
       <c r="AF21" t="s">
         <v>132</v>
       </c>
-      <c r="AG21" s="1" t="s">
+      <c r="AG21" t="s">
         <v>133</v>
       </c>
-      <c r="AH21" s="1" t="s">
+      <c r="AH21" t="s">
         <v>133</v>
       </c>
       <c r="AI21" t="s">
@@ -7012,7 +7012,7 @@
       <c r="D22" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E22" t="s">
         <v>88</v>
       </c>
       <c r="F22" s="1" t="s">
@@ -7027,22 +7027,22 @@
       <c r="I22" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J22" t="s">
-        <v>132</v>
-      </c>
-      <c r="K22" t="s">
-        <v>132</v>
+      <c r="J22" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M22" t="s">
+      <c r="M22" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O22" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P22" s="1" t="s">
@@ -7066,7 +7066,7 @@
       <c r="V22" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="W22" t="s">
+      <c r="W22" s="1" t="s">
         <v>87</v>
       </c>
       <c r="X22" t="s">
@@ -7078,19 +7078,19 @@
       <c r="Z22" t="s">
         <v>132</v>
       </c>
-      <c r="AA22" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB22" t="s">
+      <c r="AA22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB22" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC22" t="s">
         <v>91</v>
       </c>
-      <c r="AD22" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE22" t="s">
+      <c r="AD22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE22" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF22" t="s">
@@ -7102,13 +7102,13 @@
       <c r="AH22" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI22" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ22" t="s">
-        <v>87</v>
-      </c>
-      <c r="AK22" t="s">
+      <c r="AI22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK22" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AL22" s="1" t="s">
@@ -7266,7 +7266,7 @@
       <c r="D23" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E23" t="s">
         <v>88</v>
       </c>
       <c r="F23" s="1" t="s">
@@ -7281,28 +7281,28 @@
       <c r="I23" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J23" t="s">
-        <v>132</v>
-      </c>
-      <c r="K23" t="s">
-        <v>132</v>
+      <c r="J23" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M23" t="s">
+      <c r="M23" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O23" t="s">
+      <c r="O23" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P23" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q23" s="1" t="s">
+      <c r="Q23" t="s">
         <v>90</v>
       </c>
       <c r="R23" s="1" t="s">
@@ -7320,7 +7320,7 @@
       <c r="V23" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="W23" t="s">
+      <c r="W23" s="1" t="s">
         <v>87</v>
       </c>
       <c r="X23" t="s">
@@ -7332,19 +7332,19 @@
       <c r="Z23" t="s">
         <v>132</v>
       </c>
-      <c r="AA23" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB23" t="s">
+      <c r="AA23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB23" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC23" t="s">
         <v>91</v>
       </c>
-      <c r="AD23" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE23" t="s">
+      <c r="AD23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE23" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF23" t="s">
@@ -7356,10 +7356,10 @@
       <c r="AH23" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI23" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ23" t="s">
+      <c r="AI23" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ23" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AK23" t="s">
@@ -7520,7 +7520,7 @@
       <c r="D24" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" t="s">
         <v>88</v>
       </c>
       <c r="F24" s="1" t="s">
@@ -7535,28 +7535,28 @@
       <c r="I24" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J24" t="s">
-        <v>132</v>
-      </c>
-      <c r="K24" t="s">
-        <v>132</v>
+      <c r="J24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M24" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O24" t="s">
+      <c r="O24" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P24" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q24" s="1" t="s">
+      <c r="Q24" t="s">
         <v>90</v>
       </c>
       <c r="R24" s="1" t="s">
@@ -7574,7 +7574,7 @@
       <c r="V24" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="W24" t="s">
+      <c r="W24" s="1" t="s">
         <v>87</v>
       </c>
       <c r="X24" t="s">
@@ -7586,19 +7586,19 @@
       <c r="Z24" t="s">
         <v>132</v>
       </c>
-      <c r="AA24" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB24" t="s">
+      <c r="AA24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB24" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC24" t="s">
         <v>91</v>
       </c>
-      <c r="AD24" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE24" t="s">
+      <c r="AD24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE24" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF24" t="s">
@@ -7610,10 +7610,10 @@
       <c r="AH24" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI24" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ24" t="s">
+      <c r="AI24" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ24" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AK24" t="s">
@@ -7758,7 +7758,7 @@
         <v>87</v>
       </c>
       <c r="CF24" t="s">
-        <v>91</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25">
@@ -7774,7 +7774,7 @@
       <c r="D25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>88</v>
       </c>
       <c r="F25" s="1" t="s">
@@ -7789,28 +7789,28 @@
       <c r="I25" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J25" t="s">
-        <v>132</v>
-      </c>
-      <c r="K25" t="s">
-        <v>132</v>
+      <c r="J25" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M25" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O25" t="s">
+      <c r="O25" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P25" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q25" s="1" t="s">
+      <c r="Q25" t="s">
         <v>90</v>
       </c>
       <c r="R25" s="1" t="s">
@@ -7828,7 +7828,7 @@
       <c r="V25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="W25" t="s">
+      <c r="W25" s="1" t="s">
         <v>87</v>
       </c>
       <c r="X25" t="s">
@@ -7840,19 +7840,19 @@
       <c r="Z25" t="s">
         <v>132</v>
       </c>
-      <c r="AA25" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB25" t="s">
+      <c r="AA25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB25" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC25" t="s">
         <v>91</v>
       </c>
-      <c r="AD25" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE25" t="s">
+      <c r="AD25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE25" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF25" t="s">
@@ -7864,13 +7864,13 @@
       <c r="AH25" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI25" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ25" t="s">
-        <v>87</v>
-      </c>
-      <c r="AK25" t="s">
+      <c r="AI25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK25" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AL25" s="1" t="s">
@@ -8282,7 +8282,7 @@
       <c r="D27" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>88</v>
       </c>
       <c r="F27" s="1" t="s">
@@ -8297,28 +8297,28 @@
       <c r="I27" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J27" t="s">
-        <v>132</v>
-      </c>
-      <c r="K27" t="s">
-        <v>132</v>
+      <c r="J27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M27" t="s">
+      <c r="M27" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N27" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O27" t="s">
+      <c r="O27" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P27" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q27" s="1" t="s">
+      <c r="Q27" t="s">
         <v>90</v>
       </c>
       <c r="R27" s="1" t="s">
@@ -8336,7 +8336,7 @@
       <c r="V27" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="W27" t="s">
+      <c r="W27" s="1" t="s">
         <v>87</v>
       </c>
       <c r="X27" t="s">
@@ -8348,19 +8348,19 @@
       <c r="Z27" t="s">
         <v>132</v>
       </c>
-      <c r="AA27" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB27" t="s">
+      <c r="AA27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB27" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC27" t="s">
         <v>91</v>
       </c>
-      <c r="AD27" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE27" t="s">
+      <c r="AD27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE27" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF27" t="s">
@@ -8372,10 +8372,10 @@
       <c r="AH27" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI27" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ27" t="s">
+      <c r="AI27" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ27" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AK27" t="s">
@@ -8536,7 +8536,7 @@
       <c r="D28" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>88</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -8551,28 +8551,28 @@
       <c r="I28" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J28" t="s">
-        <v>132</v>
-      </c>
-      <c r="K28" t="s">
-        <v>132</v>
+      <c r="J28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M28" t="s">
+      <c r="M28" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N28" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O28" t="s">
+      <c r="O28" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P28" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q28" s="1" t="s">
+      <c r="Q28" t="s">
         <v>90</v>
       </c>
       <c r="R28" s="1" t="s">
@@ -8602,19 +8602,19 @@
       <c r="Z28" t="s">
         <v>132</v>
       </c>
-      <c r="AA28" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB28" t="s">
+      <c r="AA28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB28" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC28" t="s">
         <v>91</v>
       </c>
-      <c r="AD28" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE28" t="s">
+      <c r="AD28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE28" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF28" t="s">
@@ -8626,10 +8626,10 @@
       <c r="AH28" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI28" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ28" t="s">
+      <c r="AI28" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ28" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AK28" t="s">
@@ -8790,7 +8790,7 @@
       <c r="D29" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>88</v>
       </c>
       <c r="F29" s="1" t="s">
@@ -8805,28 +8805,28 @@
       <c r="I29" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J29" t="s">
-        <v>132</v>
-      </c>
-      <c r="K29" t="s">
-        <v>132</v>
+      <c r="J29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M29" t="s">
+      <c r="M29" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N29" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O29" t="s">
+      <c r="O29" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P29" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q29" s="1" t="s">
+      <c r="Q29" t="s">
         <v>90</v>
       </c>
       <c r="R29" s="1" t="s">
@@ -8856,19 +8856,19 @@
       <c r="Z29" t="s">
         <v>132</v>
       </c>
-      <c r="AA29" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB29" t="s">
+      <c r="AA29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB29" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC29" t="s">
         <v>91</v>
       </c>
-      <c r="AD29" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE29" t="s">
+      <c r="AD29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE29" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF29" t="s">
@@ -8880,10 +8880,10 @@
       <c r="AH29" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI29" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ29" t="s">
+      <c r="AI29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ29" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AK29" t="s">
@@ -9044,7 +9044,7 @@
       <c r="D30" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E30" t="s">
         <v>88</v>
       </c>
       <c r="F30" s="1" t="s">
@@ -9059,28 +9059,28 @@
       <c r="I30" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J30" t="s">
-        <v>132</v>
-      </c>
-      <c r="K30" t="s">
-        <v>132</v>
+      <c r="J30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M30" t="s">
+      <c r="M30" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N30" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O30" t="s">
+      <c r="O30" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P30" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q30" s="1" t="s">
+      <c r="Q30" t="s">
         <v>90</v>
       </c>
       <c r="R30" s="1" t="s">
@@ -9110,19 +9110,19 @@
       <c r="Z30" t="s">
         <v>132</v>
       </c>
-      <c r="AA30" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB30" t="s">
+      <c r="AA30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB30" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC30" t="s">
         <v>91</v>
       </c>
-      <c r="AD30" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE30" t="s">
+      <c r="AD30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE30" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF30" t="s">
@@ -9134,10 +9134,10 @@
       <c r="AH30" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI30" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ30" t="s">
+      <c r="AI30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ30" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AK30" t="s">
@@ -9298,7 +9298,7 @@
       <c r="D31" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>88</v>
       </c>
       <c r="F31" s="1" t="s">
@@ -9313,28 +9313,28 @@
       <c r="I31" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J31" t="s">
-        <v>132</v>
-      </c>
-      <c r="K31" t="s">
-        <v>132</v>
+      <c r="J31" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M31" t="s">
+      <c r="M31" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N31" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O31" t="s">
+      <c r="O31" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P31" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q31" s="1" t="s">
+      <c r="Q31" t="s">
         <v>90</v>
       </c>
       <c r="R31" s="1" t="s">
@@ -9364,19 +9364,19 @@
       <c r="Z31" t="s">
         <v>132</v>
       </c>
-      <c r="AA31" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB31" t="s">
+      <c r="AA31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB31" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC31" t="s">
         <v>91</v>
       </c>
-      <c r="AD31" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE31" t="s">
+      <c r="AD31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE31" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF31" t="s">
@@ -9388,10 +9388,10 @@
       <c r="AH31" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI31" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ31" t="s">
+      <c r="AI31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ31" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AK31" t="s">
@@ -9552,7 +9552,7 @@
       <c r="D32" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>88</v>
       </c>
       <c r="F32" s="1" t="s">
@@ -9567,28 +9567,28 @@
       <c r="I32" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J32" t="s">
-        <v>132</v>
-      </c>
-      <c r="K32" t="s">
-        <v>132</v>
+      <c r="J32" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M32" t="s">
+      <c r="M32" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N32" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O32" t="s">
+      <c r="O32" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P32" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q32" s="1" t="s">
+      <c r="Q32" t="s">
         <v>90</v>
       </c>
       <c r="R32" s="1" t="s">
@@ -9618,19 +9618,19 @@
       <c r="Z32" t="s">
         <v>132</v>
       </c>
-      <c r="AA32" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB32" t="s">
+      <c r="AA32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB32" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC32" t="s">
         <v>91</v>
       </c>
-      <c r="AD32" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE32" t="s">
+      <c r="AD32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE32" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF32" t="s">
@@ -9642,10 +9642,10 @@
       <c r="AH32" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI32" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ32" t="s">
+      <c r="AI32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ32" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AK32" t="s">
@@ -9806,7 +9806,7 @@
       <c r="D33" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>88</v>
       </c>
       <c r="F33" s="1" t="s">
@@ -9821,28 +9821,28 @@
       <c r="I33" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J33" t="s">
-        <v>132</v>
-      </c>
-      <c r="K33" t="s">
-        <v>132</v>
+      <c r="J33" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M33" t="s">
+      <c r="M33" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N33" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O33" t="s">
+      <c r="O33" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P33" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q33" s="1" t="s">
+      <c r="Q33" t="s">
         <v>90</v>
       </c>
       <c r="R33" s="1" t="s">
@@ -9872,19 +9872,19 @@
       <c r="Z33" t="s">
         <v>132</v>
       </c>
-      <c r="AA33" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB33" t="s">
+      <c r="AA33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB33" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC33" t="s">
         <v>91</v>
       </c>
-      <c r="AD33" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE33" t="s">
+      <c r="AD33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE33" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF33" t="s">
@@ -9896,10 +9896,10 @@
       <c r="AH33" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI33" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ33" t="s">
+      <c r="AI33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ33" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AK33" t="s">
@@ -10060,7 +10060,7 @@
       <c r="D34" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" t="s">
         <v>88</v>
       </c>
       <c r="F34" s="1" t="s">
@@ -10075,28 +10075,28 @@
       <c r="I34" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J34" t="s">
-        <v>132</v>
-      </c>
-      <c r="K34" t="s">
-        <v>132</v>
+      <c r="J34" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M34" t="s">
+      <c r="M34" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N34" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O34" t="s">
+      <c r="O34" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P34" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q34" s="1" t="s">
+      <c r="Q34" t="s">
         <v>90</v>
       </c>
       <c r="R34" s="1" t="s">
@@ -10126,19 +10126,19 @@
       <c r="Z34" t="s">
         <v>132</v>
       </c>
-      <c r="AA34" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB34" t="s">
+      <c r="AA34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB34" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC34" t="s">
         <v>91</v>
       </c>
-      <c r="AD34" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE34" t="s">
+      <c r="AD34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE34" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF34" t="s">
@@ -10150,10 +10150,10 @@
       <c r="AH34" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI34" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ34" t="s">
+      <c r="AI34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ34" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AK34" t="s">
@@ -10314,7 +10314,7 @@
       <c r="D35" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E35" t="s">
         <v>88</v>
       </c>
       <c r="F35" s="1" t="s">
@@ -10329,28 +10329,28 @@
       <c r="I35" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J35" t="s">
-        <v>132</v>
-      </c>
-      <c r="K35" t="s">
-        <v>132</v>
+      <c r="J35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M35" t="s">
+      <c r="M35" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N35" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O35" t="s">
+      <c r="O35" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P35" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q35" s="1" t="s">
+      <c r="Q35" t="s">
         <v>90</v>
       </c>
       <c r="R35" s="1" t="s">
@@ -10380,19 +10380,19 @@
       <c r="Z35" t="s">
         <v>132</v>
       </c>
-      <c r="AA35" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB35" t="s">
+      <c r="AA35" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB35" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC35" t="s">
         <v>91</v>
       </c>
-      <c r="AD35" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE35" t="s">
+      <c r="AD35" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE35" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF35" t="s">
@@ -10404,10 +10404,10 @@
       <c r="AH35" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI35" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ35" t="s">
+      <c r="AI35" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ35" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AK35" t="s">
@@ -10568,7 +10568,7 @@
       <c r="D36" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E36" t="s">
         <v>88</v>
       </c>
       <c r="F36" s="1" t="s">
@@ -10583,28 +10583,28 @@
       <c r="I36" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J36" t="s">
-        <v>132</v>
-      </c>
-      <c r="K36" t="s">
-        <v>132</v>
+      <c r="J36" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M36" t="s">
+      <c r="M36" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N36" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O36" t="s">
+      <c r="O36" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P36" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q36" s="1" t="s">
+      <c r="Q36" t="s">
         <v>90</v>
       </c>
       <c r="R36" s="1" t="s">
@@ -10622,7 +10622,7 @@
       <c r="V36" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="W36" t="s">
+      <c r="W36" s="1" t="s">
         <v>87</v>
       </c>
       <c r="X36" t="s">
@@ -10634,19 +10634,19 @@
       <c r="Z36" t="s">
         <v>132</v>
       </c>
-      <c r="AA36" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB36" t="s">
+      <c r="AA36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB36" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC36" t="s">
         <v>91</v>
       </c>
-      <c r="AD36" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE36" t="s">
+      <c r="AD36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE36" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF36" t="s">
@@ -10658,10 +10658,10 @@
       <c r="AH36" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI36" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ36" t="s">
+      <c r="AI36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ36" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AK36" t="s">
@@ -10822,7 +10822,7 @@
       <c r="D37" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" t="s">
         <v>88</v>
       </c>
       <c r="F37" s="1" t="s">
@@ -10837,28 +10837,28 @@
       <c r="I37" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J37" t="s">
-        <v>132</v>
-      </c>
-      <c r="K37" t="s">
-        <v>132</v>
+      <c r="J37" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M37" t="s">
+      <c r="M37" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N37" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O37" t="s">
+      <c r="O37" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P37" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q37" s="1" t="s">
+      <c r="Q37" t="s">
         <v>90</v>
       </c>
       <c r="R37" s="1" t="s">
@@ -10876,7 +10876,7 @@
       <c r="V37" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="W37" t="s">
+      <c r="W37" s="1" t="s">
         <v>87</v>
       </c>
       <c r="X37" t="s">
@@ -10888,19 +10888,19 @@
       <c r="Z37" t="s">
         <v>132</v>
       </c>
-      <c r="AA37" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB37" t="s">
+      <c r="AA37" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB37" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC37" t="s">
         <v>91</v>
       </c>
-      <c r="AD37" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE37" t="s">
+      <c r="AD37" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE37" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF37" t="s">
@@ -10912,13 +10912,13 @@
       <c r="AH37" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI37" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ37" t="s">
-        <v>87</v>
-      </c>
-      <c r="AK37" t="s">
+      <c r="AI37" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ37" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK37" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AL37" s="1" t="s">
@@ -11076,7 +11076,7 @@
       <c r="D38" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="E38" t="s">
         <v>88</v>
       </c>
       <c r="F38" s="1" t="s">
@@ -11091,28 +11091,28 @@
       <c r="I38" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J38" t="s">
-        <v>132</v>
-      </c>
-      <c r="K38" t="s">
-        <v>132</v>
+      <c r="J38" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L38" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M38" t="s">
+      <c r="M38" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N38" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O38" t="s">
+      <c r="O38" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P38" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q38" s="1" t="s">
+      <c r="Q38" t="s">
         <v>90</v>
       </c>
       <c r="R38" s="1" t="s">
@@ -11130,7 +11130,7 @@
       <c r="V38" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="W38" t="s">
+      <c r="W38" s="1" t="s">
         <v>87</v>
       </c>
       <c r="X38" t="s">
@@ -11142,19 +11142,19 @@
       <c r="Z38" t="s">
         <v>132</v>
       </c>
-      <c r="AA38" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB38" t="s">
+      <c r="AA38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB38" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC38" t="s">
         <v>91</v>
       </c>
-      <c r="AD38" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE38" t="s">
+      <c r="AD38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE38" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF38" t="s">
@@ -11166,10 +11166,10 @@
       <c r="AH38" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI38" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ38" t="s">
+      <c r="AI38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ38" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AK38" t="s">
@@ -11330,7 +11330,7 @@
       <c r="D39" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" t="s">
         <v>88</v>
       </c>
       <c r="F39" s="1" t="s">
@@ -11345,28 +11345,28 @@
       <c r="I39" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J39" t="s">
-        <v>132</v>
-      </c>
-      <c r="K39" t="s">
-        <v>132</v>
+      <c r="J39" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L39" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M39" t="s">
+      <c r="M39" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N39" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O39" t="s">
+      <c r="O39" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P39" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q39" s="1" t="s">
+      <c r="Q39" t="s">
         <v>90</v>
       </c>
       <c r="R39" s="1" t="s">
@@ -11396,19 +11396,19 @@
       <c r="Z39" t="s">
         <v>132</v>
       </c>
-      <c r="AA39" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB39" t="s">
+      <c r="AA39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB39" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC39" t="s">
         <v>91</v>
       </c>
-      <c r="AD39" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE39" t="s">
+      <c r="AD39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE39" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF39" t="s">
@@ -11420,10 +11420,10 @@
       <c r="AH39" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI39" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ39" t="s">
+      <c r="AI39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ39" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AK39" t="s">
@@ -11584,7 +11584,7 @@
       <c r="D40" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" t="s">
         <v>88</v>
       </c>
       <c r="F40" s="1" t="s">
@@ -11599,28 +11599,28 @@
       <c r="I40" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J40" t="s">
-        <v>132</v>
-      </c>
-      <c r="K40" t="s">
-        <v>132</v>
+      <c r="J40" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L40" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M40" t="s">
+      <c r="M40" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N40" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O40" t="s">
+      <c r="O40" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P40" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q40" s="1" t="s">
+      <c r="Q40" t="s">
         <v>90</v>
       </c>
       <c r="R40" s="1" t="s">
@@ -11650,19 +11650,19 @@
       <c r="Z40" t="s">
         <v>132</v>
       </c>
-      <c r="AA40" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB40" t="s">
+      <c r="AA40" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB40" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC40" t="s">
         <v>91</v>
       </c>
-      <c r="AD40" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE40" t="s">
+      <c r="AD40" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE40" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF40" t="s">
@@ -11674,10 +11674,10 @@
       <c r="AH40" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI40" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ40" t="s">
+      <c r="AI40" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ40" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AK40" t="s">
@@ -11838,7 +11838,7 @@
       <c r="D41" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" t="s">
         <v>88</v>
       </c>
       <c r="F41" s="1" t="s">
@@ -11853,22 +11853,22 @@
       <c r="I41" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J41" t="s">
-        <v>132</v>
-      </c>
-      <c r="K41" t="s">
-        <v>132</v>
+      <c r="J41" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L41" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M41" t="s">
+      <c r="M41" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N41" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O41" t="s">
+      <c r="O41" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P41" s="1" t="s">
@@ -11892,7 +11892,7 @@
       <c r="V41" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="W41" t="s">
+      <c r="W41" s="1" t="s">
         <v>87</v>
       </c>
       <c r="X41" t="s">
@@ -11904,19 +11904,19 @@
       <c r="Z41" t="s">
         <v>132</v>
       </c>
-      <c r="AA41" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB41" t="s">
+      <c r="AA41" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB41" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC41" t="s">
         <v>91</v>
       </c>
-      <c r="AD41" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE41" t="s">
+      <c r="AD41" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE41" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF41" t="s">
@@ -11928,13 +11928,13 @@
       <c r="AH41" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI41" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ41" t="s">
-        <v>87</v>
-      </c>
-      <c r="AK41" t="s">
+      <c r="AI41" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ41" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK41" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AL41" s="1" t="s">
@@ -12092,7 +12092,7 @@
       <c r="D42" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" t="s">
         <v>88</v>
       </c>
       <c r="F42" s="1" t="s">
@@ -12107,28 +12107,28 @@
       <c r="I42" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J42" t="s">
-        <v>132</v>
-      </c>
-      <c r="K42" t="s">
-        <v>132</v>
+      <c r="J42" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M42" t="s">
+      <c r="M42" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N42" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O42" t="s">
+      <c r="O42" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P42" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q42" s="1" t="s">
+      <c r="Q42" t="s">
         <v>90</v>
       </c>
       <c r="R42" s="1" t="s">
@@ -12158,19 +12158,19 @@
       <c r="Z42" t="s">
         <v>132</v>
       </c>
-      <c r="AA42" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB42" t="s">
+      <c r="AA42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB42" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC42" t="s">
         <v>91</v>
       </c>
-      <c r="AD42" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE42" t="s">
+      <c r="AD42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE42" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF42" t="s">
@@ -12182,10 +12182,10 @@
       <c r="AH42" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI42" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ42" t="s">
+      <c r="AI42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ42" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AK42" t="s">
@@ -12346,7 +12346,7 @@
       <c r="D43" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" t="s">
         <v>88</v>
       </c>
       <c r="F43" s="1" t="s">
@@ -12361,28 +12361,28 @@
       <c r="I43" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J43" t="s">
-        <v>132</v>
-      </c>
-      <c r="K43" t="s">
-        <v>132</v>
+      <c r="J43" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M43" t="s">
+      <c r="M43" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N43" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O43" t="s">
+      <c r="O43" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P43" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q43" s="1" t="s">
+      <c r="Q43" t="s">
         <v>90</v>
       </c>
       <c r="R43" s="1" t="s">
@@ -12412,19 +12412,19 @@
       <c r="Z43" t="s">
         <v>132</v>
       </c>
-      <c r="AA43" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB43" t="s">
+      <c r="AA43" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB43" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC43" t="s">
         <v>91</v>
       </c>
-      <c r="AD43" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE43" t="s">
+      <c r="AD43" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE43" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF43" t="s">
@@ -12436,10 +12436,10 @@
       <c r="AH43" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI43" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ43" t="s">
+      <c r="AI43" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ43" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AK43" t="s">
@@ -12600,7 +12600,7 @@
       <c r="D44" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" t="s">
         <v>88</v>
       </c>
       <c r="F44" s="1" t="s">
@@ -12615,28 +12615,28 @@
       <c r="I44" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J44" t="s">
-        <v>132</v>
-      </c>
-      <c r="K44" t="s">
-        <v>132</v>
+      <c r="J44" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L44" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M44" t="s">
+      <c r="M44" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N44" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O44" t="s">
+      <c r="O44" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P44" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q44" s="1" t="s">
+      <c r="Q44" t="s">
         <v>90</v>
       </c>
       <c r="R44" s="1" t="s">
@@ -12666,19 +12666,19 @@
       <c r="Z44" t="s">
         <v>132</v>
       </c>
-      <c r="AA44" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB44" t="s">
+      <c r="AA44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB44" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC44" t="s">
         <v>91</v>
       </c>
-      <c r="AD44" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE44" t="s">
+      <c r="AD44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE44" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF44" t="s">
@@ -12690,10 +12690,10 @@
       <c r="AH44" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI44" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ44" t="s">
+      <c r="AI44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ44" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AK44" t="s">
@@ -12854,7 +12854,7 @@
       <c r="D45" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E45" t="s">
         <v>88</v>
       </c>
       <c r="F45" s="1" t="s">
@@ -12869,28 +12869,28 @@
       <c r="I45" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J45" t="s">
-        <v>132</v>
-      </c>
-      <c r="K45" t="s">
-        <v>132</v>
+      <c r="J45" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M45" t="s">
+      <c r="M45" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N45" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O45" t="s">
+      <c r="O45" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P45" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q45" s="1" t="s">
+      <c r="Q45" t="s">
         <v>90</v>
       </c>
       <c r="R45" s="1" t="s">
@@ -12920,19 +12920,19 @@
       <c r="Z45" t="s">
         <v>132</v>
       </c>
-      <c r="AA45" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB45" t="s">
+      <c r="AA45" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB45" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC45" t="s">
         <v>91</v>
       </c>
-      <c r="AD45" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE45" t="s">
+      <c r="AD45" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE45" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF45" t="s">
@@ -12944,10 +12944,10 @@
       <c r="AH45" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI45" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ45" t="s">
+      <c r="AI45" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ45" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AK45" t="s">
@@ -13108,7 +13108,7 @@
       <c r="D46" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E46" t="s">
         <v>88</v>
       </c>
       <c r="F46" s="1" t="s">
@@ -13123,28 +13123,28 @@
       <c r="I46" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J46" t="s">
-        <v>132</v>
-      </c>
-      <c r="K46" t="s">
-        <v>132</v>
+      <c r="J46" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M46" t="s">
+      <c r="M46" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N46" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O46" t="s">
+      <c r="O46" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P46" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q46" s="1" t="s">
+      <c r="Q46" t="s">
         <v>90</v>
       </c>
       <c r="R46" s="1" t="s">
@@ -13174,19 +13174,19 @@
       <c r="Z46" t="s">
         <v>132</v>
       </c>
-      <c r="AA46" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB46" t="s">
+      <c r="AA46" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB46" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC46" t="s">
         <v>91</v>
       </c>
-      <c r="AD46" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE46" t="s">
+      <c r="AD46" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE46" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF46" t="s">
@@ -13198,10 +13198,10 @@
       <c r="AH46" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI46" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ46" t="s">
+      <c r="AI46" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ46" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AK46" t="s">
@@ -13362,7 +13362,7 @@
       <c r="D47" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E47" t="s">
         <v>88</v>
       </c>
       <c r="F47" s="1" t="s">
@@ -13377,22 +13377,22 @@
       <c r="I47" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J47" t="s">
-        <v>132</v>
-      </c>
-      <c r="K47" t="s">
-        <v>132</v>
+      <c r="J47" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L47" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M47" t="s">
+      <c r="M47" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N47" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O47" t="s">
+      <c r="O47" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P47" s="1" t="s">
@@ -13416,7 +13416,7 @@
       <c r="V47" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="W47" t="s">
+      <c r="W47" s="1" t="s">
         <v>87</v>
       </c>
       <c r="X47" t="s">
@@ -13428,19 +13428,19 @@
       <c r="Z47" t="s">
         <v>132</v>
       </c>
-      <c r="AA47" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB47" t="s">
+      <c r="AA47" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB47" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC47" t="s">
         <v>91</v>
       </c>
-      <c r="AD47" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE47" t="s">
+      <c r="AD47" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE47" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF47" t="s">
@@ -13452,13 +13452,13 @@
       <c r="AH47" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI47" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ47" t="s">
-        <v>87</v>
-      </c>
-      <c r="AK47" t="s">
+      <c r="AI47" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ47" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK47" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AL47" s="1" t="s">
@@ -13616,7 +13616,7 @@
       <c r="D48" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E48" t="s">
         <v>88</v>
       </c>
       <c r="F48" s="1" t="s">
@@ -13631,22 +13631,22 @@
       <c r="I48" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J48" t="s">
-        <v>132</v>
-      </c>
-      <c r="K48" t="s">
-        <v>132</v>
+      <c r="J48" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L48" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M48" t="s">
+      <c r="M48" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N48" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O48" t="s">
+      <c r="O48" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P48" s="1" t="s">
@@ -13670,7 +13670,7 @@
       <c r="V48" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="W48" t="s">
+      <c r="W48" s="1" t="s">
         <v>87</v>
       </c>
       <c r="X48" t="s">
@@ -13682,19 +13682,19 @@
       <c r="Z48" t="s">
         <v>132</v>
       </c>
-      <c r="AA48" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB48" t="s">
+      <c r="AA48" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB48" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC48" t="s">
         <v>91</v>
       </c>
-      <c r="AD48" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE48" t="s">
+      <c r="AD48" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE48" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF48" t="s">
@@ -13706,13 +13706,13 @@
       <c r="AH48" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI48" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ48" t="s">
-        <v>87</v>
-      </c>
-      <c r="AK48" t="s">
+      <c r="AI48" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ48" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK48" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AL48" s="1" t="s">
@@ -13870,7 +13870,7 @@
       <c r="D49" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E49" t="s">
         <v>88</v>
       </c>
       <c r="F49" s="1" t="s">
@@ -13885,28 +13885,28 @@
       <c r="I49" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="J49" t="s">
-        <v>132</v>
-      </c>
-      <c r="K49" t="s">
-        <v>132</v>
+      <c r="J49" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L49" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M49" t="s">
+      <c r="M49" s="1" t="s">
         <v>87</v>
       </c>
       <c r="N49" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="O49" t="s">
+      <c r="O49" s="1" t="s">
         <v>87</v>
       </c>
       <c r="P49" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="Q49" s="1" t="s">
+      <c r="Q49" t="s">
         <v>90</v>
       </c>
       <c r="R49" s="1" t="s">
@@ -13936,19 +13936,19 @@
       <c r="Z49" t="s">
         <v>132</v>
       </c>
-      <c r="AA49" t="s">
-        <v>87</v>
-      </c>
-      <c r="AB49" t="s">
+      <c r="AA49" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB49" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AC49" t="s">
         <v>91</v>
       </c>
-      <c r="AD49" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE49" t="s">
+      <c r="AD49" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE49" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AF49" t="s">
@@ -13960,10 +13960,10 @@
       <c r="AH49" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AI49" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ49" t="s">
+      <c r="AI49" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ49" s="1" t="s">
         <v>87</v>
       </c>
       <c r="AK49" t="s">

</xml_diff>